<commit_message>
Pruebas individuales sprint 3
</commit_message>
<xml_diff>
--- a/Sprint#3/Pruebas Individuales/Log pruebas individuales RF-19.xlsx
+++ b/Sprint#3/Pruebas Individuales/Log pruebas individuales RF-19.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\STACY\Documents\GitHub\SIGAB\Sprint#3\Pruebas Individuales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivane\OneDrive\Documentos\GitHub\SIGAB\Sprint#3\Pruebas Individuales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FBEAB3-DED0-4DED-9D6E-1E697DB97BF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9D5A36-88A3-46E8-9D27-FFD30C4AFED9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="RF x" sheetId="1" r:id="rId1"/>
-    <sheet name="RF y" sheetId="3" r:id="rId2"/>
+    <sheet name="RF19" sheetId="1" r:id="rId1"/>
+    <sheet name="Firmas" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>Observación</t>
   </si>
@@ -34,12 +34,6 @@
     <t>NA</t>
   </si>
   <si>
-    <t>Casos de PB suministrados por el Product Owner (Agregar)</t>
-  </si>
-  <si>
-    <t>Criterios de aceptación definidos en el RF (AZURE)</t>
-  </si>
-  <si>
     <t>Cátedra Ingeniería de Sistemas</t>
   </si>
   <si>
@@ -61,40 +55,13 @@
     <t>ID Proyecto</t>
   </si>
   <si>
-    <t>Cumple</t>
-  </si>
-  <si>
     <t>No cumple</t>
   </si>
   <si>
     <t>Log de pruebas individuales (comprobación de criterios de aceptación)</t>
   </si>
   <si>
-    <t>Que el correo de notificación tenga el formato "Se aprobó …"</t>
-  </si>
-  <si>
-    <t>Que …</t>
-  </si>
-  <si>
-    <t>El crédito debe quedar con estado….</t>
-  </si>
-  <si>
-    <t>Notificación del credito No. 25  a Maria Aguilar</t>
-  </si>
-  <si>
-    <t>Notificación del credito No. 88  a Carlos Vargas</t>
-  </si>
-  <si>
     <t>Sí cumple</t>
-  </si>
-  <si>
-    <t>Sistema XYZ</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>xxxxxxxxxxxxxx</t>
   </si>
   <si>
     <t>Jenny Ulate Montero</t>
@@ -357,7 +324,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -385,15 +352,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -408,12 +375,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -433,8 +394,74 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>34636</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>148936</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B44E006-7821-4E37-8AFA-E30248360FF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="34636"/>
+          <a:ext cx="15182850" cy="26022300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -732,21 +759,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="64.33203125" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="64.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="47" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -754,9 +781,9 @@
       <c r="E1" s="19"/>
       <c r="F1" s="3"/>
     </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
@@ -764,23 +791,23 @@
       <c r="E2" s="19"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" ht="98.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>18</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5">
         <v>9</v>
@@ -790,35 +817,35 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="12">
         <v>19</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
       <c r="E6" s="20"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" s="10">
         <v>44279</v>
@@ -828,30 +855,30 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="16" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
       <c r="E9" s="16"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>1</v>
@@ -860,108 +887,108 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>33</v>
+    <row r="11" spans="1:6" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="6"/>
       <c r="E11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>33</v>
+        <v>17</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="6"/>
     </row>
-    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="B13" s="6"/>
       <c r="C13" s="6" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
-        <v>32</v>
+    <row r="16" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="2:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="11"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="6"/>
       <c r="C19" s="6"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="11"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
@@ -980,207 +1007,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D554D50-27E8-4AAD-B616-FE3649961F4E}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="55.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="A3" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4">
-        <v>99</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-    </row>
-    <row r="4" spans="1:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="A4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" ht="21" x14ac:dyDescent="0.4">
-      <c r="A5" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="10"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="33.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-    </row>
-    <row r="18" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-    </row>
-    <row r="19" spans="1:4" ht="16.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="B9:E9"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C5:E5"/>
-  </mergeCells>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>